<commit_message>
Rerun Autotester with test cases
</commit_message>
<xml_diff>
--- a/Team05/Tests/iteration1/20-Oct-2014/ResultQBasic1A-with-clause.xlsx
+++ b/Team05/Tests/iteration1/20-Oct-2014/ResultQBasic1A-with-clause.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="15315" windowHeight="25335"/>
+    <workbookView xWindow="405" yWindow="-300" windowWidth="15315" windowHeight="25335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="67">
   <si>
     <t>name</t>
   </si>
@@ -50,6 +50,12 @@
     <t>value</t>
   </si>
   <si>
+    <t>stmtHEX</t>
+  </si>
+  <si>
+    <t>prog_lineHEX</t>
+  </si>
+  <si>
     <t>querystr</t>
   </si>
   <si>
@@ -80,9 +86,6 @@
     <t>passed</t>
   </si>
   <si>
-    <t>timeout</t>
-  </si>
-  <si>
     <t>name2</t>
   </si>
   <si>
@@ -137,7 +140,64 @@
     <t>constant c; Select BOOLEAN with c.value = 99999999999999</t>
   </si>
   <si>
-    <t>procedure p; variable v; Select p with p.procName = v.varName</t>
+    <t>stmt s; Select s with s.stmtHEX = 17</t>
+  </si>
+  <si>
+    <t>stmt s; Select s with s.stmtHEX = 99999</t>
+  </si>
+  <si>
+    <t>stmt s; Select BOOLEAN with s.stmtHEX = 23</t>
+  </si>
+  <si>
+    <t>stmt s; Select BOOLEAN with s.stmtHEX = 999999</t>
+  </si>
+  <si>
+    <t>assign a; Select a with a.stmtHEX = 12</t>
+  </si>
+  <si>
+    <t>assign a; Select a with a.stmtHEX = 27</t>
+  </si>
+  <si>
+    <t>assign a; Select BOOLEAN with a.stmtHEX = 30</t>
+  </si>
+  <si>
+    <t>assign a; Select BOOLEAN with a.stmtHEX = 19</t>
+  </si>
+  <si>
+    <t>while w; Select w with w.stmtHEX = 19</t>
+  </si>
+  <si>
+    <t>while w; Select w with w.stmtHEX = 34</t>
+  </si>
+  <si>
+    <t>while w; Select BOOLEAN with w.stmtHEX = 8</t>
+  </si>
+  <si>
+    <t>while w; Select BOOLEAN with w.stmtHEX = 25</t>
+  </si>
+  <si>
+    <t>if i; Select i with i.stmtHEX = 38</t>
+  </si>
+  <si>
+    <t>if i; Select i with i.stmtHEX = 1</t>
+  </si>
+  <si>
+    <t>if i; Select BOOLEAN with i.stmtHEX = 38</t>
+  </si>
+  <si>
+    <t>if i; Select BOOLEAN with i.stmtHEX = 15</t>
+  </si>
+  <si>
+    <t>prog_line pl; Select pl with pl.prog_lineHEX = 23</t>
+  </si>
+  <si>
+    <t>prog_line pl; Select pl with pl.prog_lineHEX = 15081992</t>
+  </si>
+  <si>
+    <t>prog_line pl; Select BOLLEAN with pl.prog_lineHEX = 1</t>
+  </si>
+  <si>
+    <t>prog_line pl; Select BOOLEAN with pl.prog_lineHEX = 15081992</t>
   </si>
   <si>
     <t>false</t>
@@ -161,85 +221,10 @@
     <t>17</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
     <t>1,10,11,12,13,14,15,16,18,19,2,20,21,22,23,24,25,26,27,28,29,3,30,31,32,33,34,35,36,37,38,39,4,40,5,6,7,8,9</t>
-  </si>
-  <si>
-    <t>stmt#</t>
-  </si>
-  <si>
-    <t>prog_line#</t>
-  </si>
-  <si>
-    <t>stmt s; Select s with s.stmt# = 17</t>
-  </si>
-  <si>
-    <t>stmt s; Select s with s.stmt# = 99999</t>
-  </si>
-  <si>
-    <t>stmt s; Select BOOLEAN with s.stmt# = 23</t>
-  </si>
-  <si>
-    <t>stmt s; Select BOOLEAN with s.stmt# = 999999</t>
-  </si>
-  <si>
-    <t>assign a; Select a with a.stmt# = 12</t>
-  </si>
-  <si>
-    <t>assign a; Select a with a.stmt# = 27</t>
-  </si>
-  <si>
-    <t>assign a; Select BOOLEAN with a.stmt# = 30</t>
-  </si>
-  <si>
-    <t>assign a; Select BOOLEAN with a.stmt# = 19</t>
-  </si>
-  <si>
-    <t>while w; Select w with w.stmt# = 19</t>
-  </si>
-  <si>
-    <t>while w; Select w with w.stmt# = 34</t>
-  </si>
-  <si>
-    <t>while w; Select BOOLEAN with w.stmt# = 8</t>
-  </si>
-  <si>
-    <t>while w; Select BOOLEAN with w.stmt# = 25</t>
-  </si>
-  <si>
-    <t>if i; Select i with i.stmt# = 38</t>
-  </si>
-  <si>
-    <t>if i; Select i with i.stmt# = 1</t>
-  </si>
-  <si>
-    <t>if i; Select BOOLEAN with i.stmt# = 38</t>
-  </si>
-  <si>
-    <t>if i; Select BOOLEAN with i.stmt# = 15</t>
-  </si>
-  <si>
-    <t>prog_line pl; Select pl with pl.prog_line# = 23</t>
-  </si>
-  <si>
-    <t>prog_line pl; Select pl with pl.prog_line# = 15081992</t>
-  </si>
-  <si>
-    <t>prog_line pl; Select BOLLEAN with pl.prog_line# = 1</t>
-  </si>
-  <si>
-    <t>prog_line pl; Select BOOLEAN with pl.prog_line# = 15081992</t>
   </si>
 </sst>
 </file>
@@ -289,7 +274,208 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -363,7 +549,6 @@
                               </xsd:element>
                               <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="exception" form="unqualified"/>
                               <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="passed" form="unqualified"/>
-                              <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="timeout" form="unqualified"/>
                             </xsd:all>
                           </xsd:complexType>
                         </xsd:element>
@@ -386,83 +571,80 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Y34" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:Y34"/>
-  <tableColumns count="25">
-    <tableColumn id="1" uniqueName="name" name="name">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:X33" tableType="xml" totalsRowShown="0" dataDxfId="0" connectionId="1">
+  <autoFilter ref="A1:X33"/>
+  <tableColumns count="24">
+    <tableColumn id="1" uniqueName="name" name="name" dataDxfId="24">
       <xmlColumnPr mapId="1" xpath="/test_results/info/name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="parsing_time_taken" name="parsing_time_taken">
+    <tableColumn id="2" uniqueName="parsing_time_taken" name="parsing_time_taken" dataDxfId="23">
       <xmlColumnPr mapId="1" xpath="/test_results/info/parsing_time_taken" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="name" name="name2">
+    <tableColumn id="3" uniqueName="name" name="name2" dataDxfId="22">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/@name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="id" name="id">
+    <tableColumn id="4" uniqueName="id" name="id" dataDxfId="21">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="procName" name="procName">
+    <tableColumn id="5" uniqueName="procName" name="procName" dataDxfId="20">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@procName" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="comment" name="comment">
+    <tableColumn id="6" uniqueName="comment" name="comment" dataDxfId="19">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@comment" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="BOOLEAN" name="BOOLEAN">
+    <tableColumn id="7" uniqueName="BOOLEAN" name="BOOLEAN" dataDxfId="18">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@BOOLEAN" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="varName" name="varName">
+    <tableColumn id="8" uniqueName="varName" name="varName" dataDxfId="17">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@varName" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="value" name="value">
+    <tableColumn id="9" uniqueName="value" name="value" dataDxfId="16">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="stmtHEX" name="stmt#">
+    <tableColumn id="10" uniqueName="stmtHEX" name="stmtHEX" dataDxfId="15">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@stmtHEX" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="prog_lineHEX" name="prog_line#">
+    <tableColumn id="11" uniqueName="prog_lineHEX" name="prog_lineHEX" dataDxfId="14">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@prog_lineHEX" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="boolean" name="boolean3">
+    <tableColumn id="12" uniqueName="boolean" name="boolean3" dataDxfId="13">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/id/@boolean" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="querystr" name="querystr">
+    <tableColumn id="13" uniqueName="querystr" name="querystr" dataDxfId="12">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/querystr" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="stuans" name="stuans">
+    <tableColumn id="14" uniqueName="stuans" name="stuans" dataDxfId="11">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/stuans" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="15" uniqueName="correct" name="correct">
+    <tableColumn id="15" uniqueName="correct" name="correct" dataDxfId="10">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/correct" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="16" uniqueName="time_taken" name="time_taken">
+    <tableColumn id="16" uniqueName="time_taken" name="time_taken" dataDxfId="9">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/time_taken" xmlDataType="double"/>
     </tableColumn>
-    <tableColumn id="17" uniqueName="missing" name="missing">
+    <tableColumn id="17" uniqueName="missing" name="missing" dataDxfId="8">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/failed/missing" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="additional" name="additional">
+    <tableColumn id="18" uniqueName="additional" name="additional" dataDxfId="7">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/failed/additional" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="19" uniqueName="expected" name="expected">
+    <tableColumn id="19" uniqueName="expected" name="expected" dataDxfId="6">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/failed/summary/expected" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="20" uniqueName="matched" name="matched">
+    <tableColumn id="20" uniqueName="matched" name="matched" dataDxfId="5">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/failed/summary/matched" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="21" uniqueName="missing" name="missing4">
+    <tableColumn id="21" uniqueName="missing" name="missing4" dataDxfId="4">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/failed/summary/missing" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="22" uniqueName="additional" name="additional5">
+    <tableColumn id="22" uniqueName="additional" name="additional5" dataDxfId="3">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/failed/summary/additional" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="23" uniqueName="exception" name="exception">
+    <tableColumn id="23" uniqueName="exception" name="exception" dataDxfId="2">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/exception" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="24" uniqueName="passed" name="passed">
+    <tableColumn id="24" uniqueName="passed" name="passed" dataDxfId="1">
       <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/passed" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="25" uniqueName="timeout" name="timeout">
-      <xmlColumnPr mapId="1" xpath="/test_results/queries/category/query/timeout" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -756,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,10 +969,9 @@
     <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -798,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -819,63 +1000,60 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="P1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="Q1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="S1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="T1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="U1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="W1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -885,17 +1063,17 @@
       </c>
       <c r="F2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="P2" s="2">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="2">
@@ -912,17 +1090,16 @@
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-    </row>
-    <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -932,7 +1109,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -940,17 +1117,16 @@
       <c r="R3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-    </row>
-    <row r="4" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -963,22 +1139,22 @@
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="P4" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="S4" s="2">
         <v>1</v>
@@ -994,17 +1170,16 @@
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-    </row>
-    <row r="5" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2">
         <v>4</v>
@@ -1017,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1025,17 +1200,16 @@
       <c r="R5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-    </row>
-    <row r="6" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2">
         <v>5</v>
@@ -1045,17 +1219,17 @@
         <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="P6" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="2">
@@ -1072,17 +1246,16 @@
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-    </row>
-    <row r="7" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2">
         <v>6</v>
@@ -1092,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1100,17 +1273,16 @@
       <c r="R7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-    </row>
-    <row r="8" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2">
         <v>7</v>
@@ -1123,22 +1295,22 @@
         <v>1</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="P8" s="2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="S8" s="2">
         <v>1</v>
@@ -1154,17 +1326,16 @@
       </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-    </row>
-    <row r="9" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
@@ -1177,17 +1348,17 @@
         <v>1</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="P9" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="2">
@@ -1204,17 +1375,16 @@
       </c>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-    </row>
-    <row r="10" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2">
         <v>9</v>
@@ -1224,17 +1394,17 @@
         <v>1</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="P10" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="2">
@@ -1251,17 +1421,16 @@
       </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-    </row>
-    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2">
         <v>10</v>
@@ -1271,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1279,17 +1448,16 @@
       <c r="R11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-    </row>
-    <row r="12" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2">
         <v>11</v>
@@ -1302,22 +1470,22 @@
         <v>1</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="P12" s="2">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="S12" s="2">
         <v>1</v>
@@ -1333,17 +1501,16 @@
       </c>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-    </row>
-    <row r="13" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2">
         <v>12</v>
@@ -1356,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1364,17 +1531,16 @@
       <c r="R13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-    </row>
-    <row r="14" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2">
         <v>13</v>
@@ -1384,20 +1550,20 @@
         <v>1</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="P14" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="S14" s="2">
         <v>1</v>
@@ -1413,17 +1579,16 @@
       </c>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-    </row>
-    <row r="15" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2">
         <v>14</v>
@@ -1433,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1441,17 +1606,16 @@
       <c r="R15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-    </row>
-    <row r="16" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2">
         <v>15</v>
@@ -1461,22 +1625,22 @@
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="P16" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="S16" s="2">
         <v>1</v>
@@ -1492,17 +1656,16 @@
       </c>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-    </row>
-    <row r="17" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="2">
         <v>16</v>
@@ -1512,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1520,17 +1683,16 @@
       <c r="R17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-    </row>
-    <row r="18" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D18" s="2">
         <v>17</v>
@@ -1540,44 +1702,24 @@
         <v>1</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="N18" s="1"/>
-      <c r="O18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P18" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="O18" s="1"/>
+      <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="2">
-        <v>1</v>
-      </c>
-      <c r="T18" s="2">
-        <v>0</v>
-      </c>
-      <c r="U18" s="2">
-        <v>1</v>
-      </c>
-      <c r="V18" s="2">
-        <v>0</v>
-      </c>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-    </row>
-    <row r="19" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
@@ -1587,28 +1729,24 @@
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="2">
-        <v>4</v>
-      </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-    </row>
-    <row r="20" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" s="2">
         <v>19</v>
@@ -1621,44 +1759,24 @@
         <v>1</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P20" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="O20" s="1"/>
+      <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="2">
-        <v>1</v>
-      </c>
-      <c r="T20" s="2">
-        <v>0</v>
-      </c>
-      <c r="U20" s="2">
-        <v>1</v>
-      </c>
-      <c r="V20" s="2">
-        <v>0</v>
-      </c>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-    </row>
-    <row r="21" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D21" s="2">
         <v>20</v>
@@ -1671,44 +1789,24 @@
         <v>1</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P21" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="O21" s="1"/>
+      <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="2">
-        <v>1</v>
-      </c>
-      <c r="T21" s="2">
-        <v>0</v>
-      </c>
-      <c r="U21" s="2">
-        <v>1</v>
-      </c>
-      <c r="V21" s="2">
-        <v>0</v>
-      </c>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-    </row>
-    <row r="22" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D22" s="2">
         <v>21</v>
@@ -1718,44 +1816,24 @@
         <v>1</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="N22" s="1"/>
-      <c r="O22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P22" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="O22" s="1"/>
+      <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="2">
-        <v>1</v>
-      </c>
-      <c r="T22" s="2">
-        <v>0</v>
-      </c>
-      <c r="U22" s="2">
-        <v>1</v>
-      </c>
-      <c r="V22" s="2">
-        <v>0</v>
-      </c>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-    </row>
-    <row r="23" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23" s="2">
         <v>22</v>
@@ -1765,28 +1843,24 @@
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="2">
-        <v>3</v>
-      </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-    </row>
-    <row r="24" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D24" s="2">
         <v>23</v>
@@ -1799,44 +1873,24 @@
         <v>1</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="N24" s="1"/>
-      <c r="O24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P24" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="O24" s="1"/>
+      <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="S24" s="2">
-        <v>1</v>
-      </c>
-      <c r="T24" s="2">
-        <v>0</v>
-      </c>
-      <c r="U24" s="2">
-        <v>1</v>
-      </c>
-      <c r="V24" s="2">
-        <v>0</v>
-      </c>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-    </row>
-    <row r="25" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="2">
         <v>24</v>
@@ -1849,44 +1903,24 @@
         <v>1</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="N25" s="1"/>
-      <c r="O25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P25" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="O25" s="1"/>
+      <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="2">
-        <v>1</v>
-      </c>
-      <c r="T25" s="2">
-        <v>0</v>
-      </c>
-      <c r="U25" s="2">
-        <v>1</v>
-      </c>
-      <c r="V25" s="2">
-        <v>0</v>
-      </c>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-    </row>
-    <row r="26" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D26" s="2">
         <v>25</v>
@@ -1896,44 +1930,24 @@
         <v>1</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="N26" s="1"/>
-      <c r="O26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P26" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="O26" s="1"/>
+      <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-      <c r="S26" s="2">
-        <v>1</v>
-      </c>
-      <c r="T26" s="2">
-        <v>0</v>
-      </c>
-      <c r="U26" s="2">
-        <v>1</v>
-      </c>
-      <c r="V26" s="2">
-        <v>0</v>
-      </c>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-    </row>
-    <row r="27" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B27" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D27" s="2">
         <v>26</v>
@@ -1943,28 +1957,24 @@
         <v>1</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="2">
-        <v>3</v>
-      </c>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-    </row>
-    <row r="28" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B28" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D28" s="2">
         <v>27</v>
@@ -1977,44 +1987,24 @@
         <v>1</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="N28" s="1"/>
-      <c r="O28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P28" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="O28" s="1"/>
+      <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
-      <c r="S28" s="2">
-        <v>1</v>
-      </c>
-      <c r="T28" s="2">
-        <v>0</v>
-      </c>
-      <c r="U28" s="2">
-        <v>1</v>
-      </c>
-      <c r="V28" s="2">
-        <v>0</v>
-      </c>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-    </row>
-    <row r="29" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B29" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D29" s="2">
         <v>28</v>
@@ -2027,44 +2017,24 @@
         <v>1</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="N29" s="1"/>
-      <c r="O29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P29" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="O29" s="1"/>
+      <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
-      <c r="S29" s="2">
-        <v>1</v>
-      </c>
-      <c r="T29" s="2">
-        <v>0</v>
-      </c>
-      <c r="U29" s="2">
-        <v>1</v>
-      </c>
-      <c r="V29" s="2">
-        <v>0</v>
-      </c>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-    </row>
-    <row r="30" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B30" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D30" s="2">
         <v>29</v>
@@ -2074,17 +2044,17 @@
         <v>1</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="P30" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30" s="2">
@@ -2101,17 +2071,16 @@
       </c>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-    </row>
-    <row r="31" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D31" s="2">
         <v>30</v>
@@ -2121,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2132,17 +2101,16 @@
       <c r="R31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-    </row>
-    <row r="32" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B32" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D32" s="2">
         <v>31</v>
@@ -2155,17 +2123,17 @@
         <v>1</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="P32" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="2">
@@ -2182,17 +2150,16 @@
       </c>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-    </row>
-    <row r="33" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D33" s="2">
         <v>32</v>
@@ -2205,17 +2172,17 @@
         <v>1</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="P33" s="2">
         <v>4</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="R33" s="1"/>
       <c r="S33" s="2">
@@ -2232,43 +2199,20 @@
       </c>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-    </row>
-    <row r="34" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="2">
-        <v>8</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="2">
-        <v>33</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="H34" s="2">
-        <v>1</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-    </row>
+    </row>
+    <row r="34" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>